<commit_message>
Combinaciones de Peronos, clasificacion R, completada
</commit_message>
<xml_diff>
--- a/Casos_Combinaciones_Pernos.xlsx
+++ b/Casos_Combinaciones_Pernos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc67b48cbbb67f25/robotica2025/Robotica-2025/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Desktop\UAM - StvM\Robotica-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{F1DAE5DB-1062-455E-BA4F-B95B0C02A8C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77A9D502-282E-4A91-8370-2658F9F13AC9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A210A12-7D3B-4910-AFF2-7AA98DE30C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2776C83B-0625-4CDA-B8B2-054A15CA8883}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2776C83B-0625-4CDA-B8B2-054A15CA8883}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="19">
   <si>
     <t>First</t>
   </si>
@@ -546,13 +546,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB649018-430E-41A0-A838-956B3F9B8B8C}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
         <v>17</v>
       </c>
@@ -574,7 +574,7 @@
       <c r="O1" s="9"/>
       <c r="P1" s="9"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -615,7 +615,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -653,7 +653,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -667,7 +667,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -705,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -746,7 +746,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
@@ -784,7 +784,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -798,7 +798,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
@@ -836,7 +836,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -877,7 +877,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
@@ -915,7 +915,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -929,7 +929,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -967,7 +967,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1060,7 +1060,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -1098,7 +1098,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>18</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1191,7 +1191,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
@@ -1229,7 +1229,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
       <c r="B28" s="1" t="s">
         <v>13</v>
       </c>
@@ -1267,7 +1270,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
         <v>0</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1319,7 +1322,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Completando todas las combinaciones de A
</commit_message>
<xml_diff>
--- a/Casos_Combinaciones_Pernos.xlsx
+++ b/Casos_Combinaciones_Pernos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Desktop\UAM - StvM\Robotica-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E117B3-B529-4EE6-9FF1-6B08D8ADE280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47DFCCFF-9DE7-437D-998B-57C9CDB21EFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2776C83B-0625-4CDA-B8B2-054A15CA8883}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="16">
   <si>
     <t>First</t>
   </si>
@@ -199,7 +199,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -208,6 +208,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -564,26 +565,26 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="F1" s="9" t="s">
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="F1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="J1" s="10" t="s">
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="J1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="N1" s="11" t="s">
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="N1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1042,7 +1043,7 @@
       <c r="D18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="1" t="s">
@@ -1190,7 +1191,7 @@
       <c r="D23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="E23" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -1338,6 +1339,9 @@
       <c r="D28" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E28" s="13" t="s">
+        <v>13</v>
+      </c>
       <c r="F28" s="1" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Completando la combinacion V2
</commit_message>
<xml_diff>
--- a/Casos_Combinaciones_Pernos.xlsx
+++ b/Casos_Combinaciones_Pernos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Desktop\UAM - StvM\Robotica-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4B0B8E-1594-4187-A124-8D4EBA6A179D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7303723-242E-450A-841C-8A2F35F5A144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2776C83B-0625-4CDA-B8B2-054A15CA8883}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="16">
   <si>
     <t>First</t>
   </si>
@@ -571,7 +571,7 @@
   <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,6 +774,9 @@
       <c r="H8" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="I8" s="14" t="s">
+        <v>13</v>
+      </c>
       <c r="J8" s="1" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
se revisaron las combinaciones
</commit_message>
<xml_diff>
--- a/Casos_Combinaciones_Pernos.xlsx
+++ b/Casos_Combinaciones_Pernos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Desktop\UAM - StvM\Robotica-2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cc67b48cbbb67f25/robotica2025/Robotica-2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7303723-242E-450A-841C-8A2F35F5A144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{C7303723-242E-450A-841C-8A2F35F5A144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7279CC04-DC39-438B-AD55-C73F27E5FF08}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2776C83B-0625-4CDA-B8B2-054A15CA8883}"/>
+    <workbookView xWindow="300" yWindow="1920" windowWidth="17124" windowHeight="8880" xr2:uid="{2776C83B-0625-4CDA-B8B2-054A15CA8883}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -107,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,6 +162,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -210,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -220,6 +226,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -232,8 +239,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,36 +577,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB649018-430E-41A0-A838-956B3F9B8B8C}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="190" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="F1" s="10" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="F1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="J1" s="11" t="s">
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="J1" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="N1" s="12" t="s">
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="N1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -623,7 +630,7 @@
       <c r="H3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="9" t="s">
         <v>13</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -645,7 +652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,7 +690,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -697,7 +704,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -735,7 +742,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -749,8 +756,8 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -774,7 +781,7 @@
       <c r="H8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="9" t="s">
         <v>13</v>
       </c>
       <c r="J8" s="1" t="s">
@@ -796,7 +803,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
         <v>0</v>
       </c>
@@ -834,7 +841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -848,7 +855,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
@@ -886,7 +893,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -900,7 +907,7 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -944,7 +951,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
@@ -982,7 +989,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -996,7 +1003,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1034,7 +1041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1048,8 +1055,8 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1092,7 +1099,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1111,6 +1118,7 @@
       <c r="H19" s="5">
         <v>3</v>
       </c>
+      <c r="I19" s="14"/>
       <c r="J19" s="1" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1138,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1144,7 +1152,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -1182,7 +1190,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1196,7 +1204,7 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1240,7 +1248,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
@@ -1278,7 +1286,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1292,7 +1300,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
@@ -1330,7 +1338,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1344,7 +1352,7 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1357,7 +1365,7 @@
       <c r="D28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="8" t="s">
         <v>13</v>
       </c>
       <c r="F28" s="1" t="s">
@@ -1388,7 +1396,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>0</v>
       </c>
@@ -1426,7 +1434,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1440,7 +1448,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Comprobando las combinaciones, por la 5ta
</commit_message>
<xml_diff>
--- a/Casos_Combinaciones_Pernos.xlsx
+++ b/Casos_Combinaciones_Pernos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Desktop\UAM - StvM\Robotica-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{927F7CD0-D655-4B60-AF6A-5329F783ACCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90D548F3-1352-4A53-932A-7E6079C1AFA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2776C83B-0625-4CDA-B8B2-054A15CA8883}"/>
   </bookViews>
@@ -219,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -231,6 +231,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -243,10 +245,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,29 +588,29 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="F1" s="12" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="F1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="J1" s="13" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="J1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="N1" s="14" t="s">
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="N1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -659,7 +657,7 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+      <c r="A4" s="11">
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -700,7 +698,6 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="15"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -715,7 +712,6 @@
       <c r="P5" s="1"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="15"/>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -754,7 +750,6 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -769,7 +764,7 @@
       <c r="P7" s="2"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
@@ -816,7 +811,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="17">
+      <c r="A9" s="10">
         <v>1.1689814814814816E-3</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -857,7 +852,6 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="15"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -872,7 +866,6 @@
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="15"/>
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
@@ -911,7 +904,6 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -926,7 +918,7 @@
       <c r="P12" s="2"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -970,7 +962,7 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="17">
+      <c r="A14" s="10">
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -1011,7 +1003,6 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1026,7 +1017,6 @@
       <c r="P15" s="1"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="15"/>
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1065,7 +1055,6 @@
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1080,7 +1069,7 @@
       <c r="P17" s="2"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="12" t="s">
         <v>13</v>
       </c>
       <c r="B18" s="1" t="s">

</xml_diff>

<commit_message>
Combinacion A2 probada y A3 sin cronometrar
</commit_message>
<xml_diff>
--- a/Casos_Combinaciones_Pernos.xlsx
+++ b/Casos_Combinaciones_Pernos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Desktop\UAM - StvM\Robotica-2025\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naole\Downloads\rboooooo\Robotica-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2194C77-B869-44EE-ADB8-F23E20674ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F273C8-50FC-490D-8F2A-450582B128C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2776C83B-0625-4CDA-B8B2-054A15CA8883}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2776C83B-0625-4CDA-B8B2-054A15CA8883}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,24 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={8F442683-5DC8-4D91-89F7-36CDD1844830}</author>
+  </authors>
+  <commentList>
+    <comment ref="E8" authorId="0" shapeId="0" xr:uid="{8F442683-5DC8-4D91-89F7-36CDD1844830}">
+      <text>
+        <t>[Comentario encadenado]
+Tu versión de Excel te permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Se estan probando con el rojo</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -93,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +126,12 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="11">
@@ -219,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -246,7 +270,6 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -262,6 +285,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="johaneris Avalos" id="{1554E87A-5DE1-4817-9E81-4FAAFE41DBD9}" userId="cc67b48cbbb67f25" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -579,17 +608,25 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="E8" dT="2025-07-21T14:57:24.19" personId="{1554E87A-5DE1-4817-9E81-4FAAFE41DBD9}" id="{8F442683-5DC8-4D91-89F7-36CDD1844830}">
+    <text>Se estan probando con el rojo</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB649018-430E-41A0-A838-956B3F9B8B8C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB649018-430E-41A0-A838-956B3F9B8B8C}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E8" zoomScale="154" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="154" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B1" s="14" t="s">
         <v>11</v>
       </c>
@@ -611,7 +648,7 @@
       <c r="O1" s="17"/>
       <c r="P1" s="17"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>12</v>
       </c>
@@ -648,7 +685,7 @@
       <c r="L3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -661,7 +698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="11">
         <v>1.3888888888888889E-3</v>
       </c>
@@ -705,7 +742,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -719,7 +756,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -757,7 +794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -771,7 +808,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>12</v>
       </c>
@@ -784,7 +821,7 @@
       <c r="D8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="13" t="s">
         <v>12</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -808,7 +845,7 @@
       <c r="L8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M8" s="18" t="s">
+      <c r="M8" s="9" t="s">
         <v>12</v>
       </c>
       <c r="N8" s="1" t="s">
@@ -821,7 +858,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <v>1.1689814814814816E-3</v>
       </c>
@@ -862,10 +899,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
+      <c r="E10" s="10">
+        <v>1.3194444444444445E-3</v>
+      </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -876,7 +916,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
@@ -914,7 +954,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -928,7 +968,7 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>12</v>
       </c>
@@ -975,7 +1015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <v>1.3888888888888889E-3</v>
       </c>
@@ -1019,7 +1059,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -1035,7 +1075,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1073,7 +1113,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1087,7 +1127,7 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
         <v>12</v>
       </c>
@@ -1112,7 +1152,7 @@
       <c r="H18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="18" t="s">
+      <c r="I18" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J18" s="1" t="s">
@@ -1134,7 +1174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="10">
         <v>1.3078703703703703E-3</v>
       </c>
@@ -1175,7 +1215,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1189,7 +1229,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -1227,7 +1267,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1241,7 +1281,7 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="12" t="s">
         <v>12</v>
       </c>
@@ -1266,7 +1306,7 @@
       <c r="H23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I23" s="18" t="s">
+      <c r="I23" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J23" s="1" t="s">
@@ -1288,7 +1328,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="10">
         <v>1.4004629629629629E-3</v>
       </c>
@@ -1329,7 +1369,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1343,7 +1383,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
@@ -1381,7 +1421,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1395,7 +1435,7 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A28" s="12" t="s">
         <v>12</v>
       </c>
@@ -1420,7 +1460,7 @@
       <c r="H28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I28" s="18" t="s">
+      <c r="I28" s="9" t="s">
         <v>12</v>
       </c>
       <c r="J28" s="1" t="s">
@@ -1442,7 +1482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A29" s="10">
         <v>1.4120370370370369E-3</v>
       </c>
@@ -1483,7 +1523,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1497,7 +1537,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>1</v>
       </c>
@@ -1543,5 +1583,6 @@
     <mergeCell ref="N1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Preparado para la competencia...
</commit_message>
<xml_diff>
--- a/Casos_Combinaciones_Pernos.xlsx
+++ b/Casos_Combinaciones_Pernos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gabri\OneDrive\Desktop\UAM - StvM\Robotica-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8277DD-EB94-440E-BFAA-4531D2E2500A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37FB9FD8-0D98-444D-AE42-12F22065AD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2776C83B-0625-4CDA-B8B2-054A15CA8883}"/>
+    <workbookView xWindow="14295" yWindow="7740" windowWidth="14610" windowHeight="7845" xr2:uid="{2776C83B-0625-4CDA-B8B2-054A15CA8883}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
     <comment ref="E8" authorId="0" shapeId="0" xr:uid="{8F442683-5DC8-4D91-89F7-36CDD1844830}">
       <text>
         <t>[Comentario encadenado]
-Tu versión de Excel te permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
 Comentario:
     Se estan probando con el rojo</t>
       </text>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="22">
   <si>
     <t>First</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>probando</t>
+  </si>
+  <si>
+    <t>no v a</t>
   </si>
 </sst>
 </file>
@@ -252,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -266,6 +269,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -281,13 +290,6 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -638,35 +640,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB649018-430E-41A0-A838-956B3F9B8B8C}">
   <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="154" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="F1" s="14" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="F1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="J1" s="15" t="s">
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="J1" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="N1" s="16" t="s">
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="N1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
@@ -710,7 +712,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="10"/>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -750,7 +752,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -764,7 +766,7 @@
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -802,7 +804,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -816,7 +818,7 @@
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -864,8 +866,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="19" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
@@ -877,7 +879,7 @@
       <c r="D9" s="4">
         <v>9</v>
       </c>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="14" t="s">
         <v>18</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -908,12 +910,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A10" s="17"/>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="19"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="19"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -924,7 +926,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
@@ -962,7 +964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -976,7 +978,7 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>15</v>
       </c>
@@ -990,7 +992,7 @@
         <v>3</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>6</v>
@@ -1011,7 +1013,7 @@
       <c r="L13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M13" s="20" t="s">
+      <c r="M13" s="8" t="s">
         <v>19</v>
       </c>
       <c r="N13" s="1" t="s">
@@ -1024,7 +1026,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>18</v>
       </c>
@@ -1037,9 +1039,7 @@
       <c r="D14" s="4">
         <v>9</v>
       </c>
-      <c r="E14" s="18" t="s">
-        <v>17</v>
-      </c>
+      <c r="E14" s="13"/>
       <c r="F14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1069,11 +1069,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="18"/>
+      <c r="E15" s="13"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1086,7 +1086,7 @@
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -1138,7 +1138,7 @@
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="1" t="s">
         <v>7</v>
@@ -1179,7 +1179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
       <c r="B19" s="1" t="s">
         <v>0</v>
@@ -1218,7 +1218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -1232,7 +1232,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
         <v>1</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1284,7 +1284,7 @@
       <c r="O22" s="2"/>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="1" t="s">
         <v>8</v>
@@ -1325,7 +1325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
       <c r="B24" s="1" t="s">
         <v>0</v>
@@ -1367,7 +1367,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
@@ -1381,7 +1381,7 @@
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
         <v>1</v>
       </c>
@@ -1419,7 +1419,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1433,7 +1433,7 @@
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="1" t="s">
         <v>9</v>
@@ -1476,7 +1476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="9"/>
       <c r="B29" s="1" t="s">
         <v>0</v>
@@ -1515,7 +1515,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
@@ -1529,7 +1529,7 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
         <v>1</v>
       </c>
@@ -1569,13 +1569,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="A9:A10"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="E9:E10"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="J1:L1"/>
-    <mergeCell ref="N1:P1"/>
-    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>